<commit_message>
error destination before position
</commit_message>
<xml_diff>
--- a/MouvementsData.xlsx
+++ b/MouvementsData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Rang</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>MIC</t>
-  </si>
-  <si>
-    <t>stock</t>
   </si>
 </sst>
 </file>
@@ -536,7 +533,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -610,8 +607,8 @@
       <c r="C3" s="3">
         <v>22650</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>48</v>
+      <c r="D3" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
@@ -647,8 +644,8 @@
       <c r="C5" s="3">
         <v>21750</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>48</v>
+      <c r="D5" s="5">
+        <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>19</v>
@@ -664,8 +661,8 @@
       <c r="C6" s="3">
         <v>15880</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>48</v>
+      <c r="D6" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
@@ -724,8 +721,8 @@
       <c r="C9" s="3">
         <v>15020</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>48</v>
+      <c r="D9" s="5">
+        <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>19</v>
@@ -741,8 +738,8 @@
       <c r="C10" s="3">
         <v>25250</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>48</v>
+      <c r="D10" s="5">
+        <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>19</v>
@@ -758,8 +755,8 @@
       <c r="C11" s="3">
         <v>17200</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>48</v>
+      <c r="D11" s="5">
+        <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>19</v>
@@ -775,8 +772,8 @@
       <c r="C12" s="3">
         <v>22650</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>48</v>
+      <c r="D12" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
@@ -789,8 +786,8 @@
       <c r="C13" s="3">
         <v>14700</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>48</v>
+      <c r="D13" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
@@ -803,8 +800,8 @@
       <c r="C14" s="3">
         <v>21750</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>48</v>
+      <c r="D14" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
@@ -863,8 +860,8 @@
       <c r="C17" s="3">
         <v>22150</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>48</v>
+      <c r="D17" s="5">
+        <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>19</v>
@@ -880,8 +877,8 @@
       <c r="C18" s="3">
         <v>22150</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>48</v>
+      <c r="D18" s="5">
+        <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>19</v>
@@ -897,8 +894,8 @@
       <c r="C19" s="3">
         <v>15020</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>48</v>
+      <c r="D19" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
@@ -911,8 +908,8 @@
       <c r="C20" s="3">
         <v>25250</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>48</v>
+      <c r="D20" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1">
@@ -948,8 +945,8 @@
       <c r="C22" s="3">
         <v>22650</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>48</v>
+      <c r="D22" s="5">
+        <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>19</v>
@@ -965,8 +962,8 @@
       <c r="C23" s="3">
         <v>15880</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>48</v>
+      <c r="D23" s="5">
+        <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>19</v>
@@ -982,8 +979,8 @@
       <c r="C24" s="3">
         <v>25120</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>48</v>
+      <c r="D24" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
@@ -996,8 +993,8 @@
       <c r="C25" s="3">
         <v>22150</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>48</v>
+      <c r="D25" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
@@ -1010,8 +1007,8 @@
       <c r="C26" s="3">
         <v>15020</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>48</v>
+      <c r="D26" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
@@ -1024,8 +1021,8 @@
       <c r="C27" s="3">
         <v>25120</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>48</v>
+      <c r="D27" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1">
@@ -1038,8 +1035,8 @@
       <c r="C28" s="3">
         <v>22150</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>48</v>
+      <c r="D28" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
@@ -1052,8 +1049,8 @@
       <c r="C29" s="3">
         <v>15020</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>48</v>
+      <c r="D29" s="5">
+        <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>19</v>
@@ -1069,8 +1066,8 @@
       <c r="C30" s="3">
         <v>25250</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>48</v>
+      <c r="D30" s="5">
+        <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>19</v>
@@ -1086,8 +1083,8 @@
       <c r="C31" s="3">
         <v>17200</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>48</v>
+      <c r="D31" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1">
@@ -1100,8 +1097,8 @@
       <c r="C32" s="3">
         <v>22650</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>48</v>
+      <c r="D32" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1">
@@ -1114,8 +1111,8 @@
       <c r="C33" s="3">
         <v>14700</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>48</v>
+      <c r="D33" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1">

</xml_diff>